<commit_message>
Started testing the game from the ground up.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/raid-bosses.xlsx
+++ b/resources/data-imports/Monsters/raid-bosses.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">2000000000-4000000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface</t>
   </si>
 </sst>
 </file>
@@ -251,8 +254,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,334 +283,334 @@
   <dimension ref="A1:AW2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="AW2"/>
+      <selection pane="topLeft" activeCell="AO3" activeCellId="0" sqref="AO3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="8.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="32.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="25.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="26.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="30.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="26.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="42" style="0" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="45" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="48" style="0" width="29.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="8.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="8.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="32.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="21.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="26.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="30.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="21.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="26.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="42" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="45" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="48" style="1" width="29.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="0" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="0" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="0" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="0" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="0" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="0" t="s">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="0" t="s">
+      <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="0" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>369</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>8000000000</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>8000000000</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>8000000000</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>8000000000</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>8000000000</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>8000000000</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>8000000000</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>4000000000</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" s="0" t="n">
+      <c r="K2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="n">
         <v>9999</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <v>150000</v>
       </c>
-      <c r="V2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="W2" s="0" t="n">
+      <c r="V2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="n">
         <v>1000000000000</v>
       </c>
-      <c r="X2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="0" t="s">
+      <c r="X2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="Z2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AA2" s="1" t="n">
         <v>250000000</v>
       </c>
-      <c r="AB2" s="0" t="n">
+      <c r="AB2" s="1" t="n">
         <v>125000000</v>
       </c>
-      <c r="AC2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="0" t="n">
+      <c r="AC2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ2" s="1" t="n">
         <v>0.35</v>
       </c>
-      <c r="AR2" s="0" t="n">
+      <c r="AR2" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="AS2" s="0" t="n">
+      <c r="AS2" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="AU2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="0" t="n">
+      <c r="AU2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1" t="n">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>